<commit_message>
Added testcases to com.supermarket
</commit_message>
<xml_diff>
--- a/com.supermarket/src/main/resources/ExcelFiles/Push Notification.xlsx
+++ b/com.supermarket/src/main/resources/ExcelFiles/Push Notification.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiran\git\com.supermarket\com.supermarket\src\main\resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45B06D59-9B12-474E-B829-4FC93626BAC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54239C9B-394A-4078-A90C-ED25D52A1B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5379A4E3-C407-4420-8640-B3357ED3C5AB}"/>
   </bookViews>
@@ -33,12 +33,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>abcd</t>
-  </si>
-  <si>
-    <t>information</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Vegetables</t>
+  </si>
+  <si>
+    <t>Fresh Vegetables</t>
+  </si>
+  <si>
+    <t>Fruits</t>
+  </si>
+  <si>
+    <t>Fresh Fruits</t>
+  </si>
+  <si>
+    <t>Bakery</t>
+  </si>
+  <si>
+    <t>Homemade items</t>
   </si>
 </sst>
 </file>
@@ -390,15 +402,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82A66FB5-40E5-4257-BE78-4C91FFD28FB9}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -409,6 +422,22 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>